<commit_message>
Completed login functionality with data driven
</commit_message>
<xml_diff>
--- a/src/main/java/com/vtiger/qa/testdata/Vtiger TestData.xlsx
+++ b/src/main/java/com/vtiger/qa/testdata/Vtiger TestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -15,9 +15,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>suresh@getnada.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>ganesh@getnada.com</t>
+  </si>
+  <si>
+    <t>rahul.chinchore@gmail.com</t>
+  </si>
+  <si>
+    <t>Login - Vtiger</t>
+  </si>
+  <si>
+    <t>expected_title</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Vtiger Buzz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +60,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,13 +92,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,13 +402,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>